<commit_message>
Fix bug in ExprSubLevel4 rule of the grammar
</commit_message>
<xml_diff>
--- a/docs/ParsingTable.xlsx
+++ b/docs/ParsingTable.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="256">
   <si>
     <t xml:space="preserve">ident</t>
   </si>
@@ -586,12 +586,12 @@
     <t xml:space="preserve">r58</t>
   </si>
   <si>
+    <t xml:space="preserve">s113 / r58</t>
+  </si>
+  <si>
     <t xml:space="preserve">r60</t>
   </si>
   <si>
-    <t xml:space="preserve">s113 / r60</t>
-  </si>
-  <si>
     <t xml:space="preserve">s114</t>
   </si>
   <si>
@@ -706,7 +706,13 @@
     <t xml:space="preserve">r56</t>
   </si>
   <si>
+    <t xml:space="preserve">s113 / r56</t>
+  </si>
+  <si>
     <t xml:space="preserve">r57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s113 / r57</t>
   </si>
   <si>
     <t xml:space="preserve">r59</t>
@@ -928,7 +934,7 @@
   <dimension ref="A1:BW1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8543,7 +8549,7 @@
         <v>187</v>
       </c>
       <c r="AH82" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AI82" s="4"/>
       <c r="AJ82" s="4"/>
@@ -8605,24 +8611,24 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
       <c r="G83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I83" s="4"/>
       <c r="J83" s="4"/>
@@ -8632,46 +8638,46 @@
       <c r="N83" s="4"/>
       <c r="O83" s="4"/>
       <c r="P83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Q83" s="4"/>
       <c r="R83" s="4"/>
       <c r="S83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="T83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="U83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="V83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="W83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="X83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Y83" s="4"/>
       <c r="Z83" s="4"/>
       <c r="AA83" s="4"/>
       <c r="AB83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AC83" s="4"/>
       <c r="AD83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AE83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AF83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AG83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AH83" s="3" t="s">
         <v>189</v>
@@ -8683,28 +8689,28 @@
         <v>191</v>
       </c>
       <c r="AK83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AL83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AM83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AN83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AO83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AP83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AQ83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AR83" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AS83" s="4"/>
       <c r="AT83" s="4"/>
@@ -12354,9 +12360,11 @@
       <c r="BP115" s="4"/>
       <c r="BQ115" s="4"/>
       <c r="BR115" s="4"/>
-      <c r="BS115" s="4"/>
+      <c r="BS115" s="3" t="n">
+        <v>134</v>
+      </c>
       <c r="BT115" s="3" t="n">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="BU115" s="3" t="n">
         <v>84</v>
@@ -14381,7 +14389,7 @@
         <v>227</v>
       </c>
       <c r="AH134" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AI134" s="4"/>
       <c r="AJ134" s="4"/>
@@ -14443,24 +14451,24 @@
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E135" s="4"/>
       <c r="F135" s="4"/>
       <c r="G135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I135" s="4"/>
       <c r="J135" s="4"/>
@@ -14470,75 +14478,75 @@
       <c r="N135" s="4"/>
       <c r="O135" s="4"/>
       <c r="P135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="Q135" s="4"/>
       <c r="R135" s="4"/>
       <c r="S135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="T135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="U135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="V135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="W135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="X135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="Y135" s="4"/>
       <c r="Z135" s="4"/>
       <c r="AA135" s="4"/>
       <c r="AB135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AC135" s="4"/>
       <c r="AD135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AE135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AF135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AG135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AH135" s="3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="AI135" s="4"/>
       <c r="AJ135" s="4"/>
       <c r="AK135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AL135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AM135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AN135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AO135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AP135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AQ135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AR135" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AS135" s="4"/>
       <c r="AT135" s="4"/>
@@ -14574,24 +14582,24 @@
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="E136" s="4"/>
       <c r="F136" s="4"/>
       <c r="G136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="H136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="I136" s="4"/>
       <c r="J136" s="4"/>
@@ -14601,75 +14609,79 @@
       <c r="N136" s="4"/>
       <c r="O136" s="4"/>
       <c r="P136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="Q136" s="4"/>
       <c r="R136" s="4"/>
       <c r="S136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="T136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="U136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="V136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="W136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="X136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="Y136" s="4"/>
       <c r="Z136" s="4"/>
       <c r="AA136" s="4"/>
       <c r="AB136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AC136" s="4"/>
       <c r="AD136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AE136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AF136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AG136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AH136" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="AI136" s="4"/>
-      <c r="AJ136" s="4"/>
+        <v>231</v>
+      </c>
+      <c r="AI136" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="AJ136" s="3" t="s">
+        <v>191</v>
+      </c>
       <c r="AK136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AL136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AM136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AN136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AO136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AP136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AQ136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AR136" s="3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AS136" s="4"/>
       <c r="AT136" s="4"/>
@@ -14705,24 +14717,24 @@
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E137" s="4"/>
       <c r="F137" s="4"/>
       <c r="G137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="I137" s="4"/>
       <c r="J137" s="4"/>
@@ -14732,79 +14744,79 @@
       <c r="N137" s="4"/>
       <c r="O137" s="4"/>
       <c r="P137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="Q137" s="4"/>
       <c r="R137" s="4"/>
       <c r="S137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="T137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="U137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="V137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="W137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="X137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="Y137" s="4"/>
       <c r="Z137" s="4"/>
       <c r="AA137" s="4"/>
       <c r="AB137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AC137" s="4"/>
       <c r="AD137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AE137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AF137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AG137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AH137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AI137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AJ137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AK137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AL137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AM137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AN137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AO137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AP137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AQ137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AR137" s="3" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AS137" s="4"/>
       <c r="AT137" s="4"/>
@@ -14840,24 +14852,24 @@
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E138" s="4"/>
       <c r="F138" s="4"/>
       <c r="G138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="I138" s="4"/>
       <c r="J138" s="4"/>
@@ -14867,79 +14879,79 @@
       <c r="N138" s="4"/>
       <c r="O138" s="4"/>
       <c r="P138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="Q138" s="4"/>
       <c r="R138" s="4"/>
       <c r="S138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="T138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="U138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="V138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="W138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="X138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="Y138" s="4"/>
       <c r="Z138" s="4"/>
       <c r="AA138" s="4"/>
       <c r="AB138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AC138" s="4"/>
       <c r="AD138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AE138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AF138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AG138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AH138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AI138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AJ138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AK138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AL138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AM138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AN138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AO138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AP138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AQ138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AR138" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AS138" s="4"/>
       <c r="AT138" s="4"/>
@@ -14978,7 +14990,7 @@
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
       <c r="D139" s="3" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E139" s="4"/>
       <c r="F139" s="4"/>
@@ -15189,24 +15201,24 @@
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E141" s="4"/>
       <c r="F141" s="4"/>
       <c r="G141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="I141" s="4"/>
       <c r="J141" s="4"/>
@@ -15216,79 +15228,79 @@
       <c r="N141" s="4"/>
       <c r="O141" s="4"/>
       <c r="P141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="Q141" s="4"/>
       <c r="R141" s="4"/>
       <c r="S141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="T141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="U141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="V141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="W141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="X141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="Y141" s="4"/>
       <c r="Z141" s="4"/>
       <c r="AA141" s="4"/>
       <c r="AB141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AC141" s="4"/>
       <c r="AD141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AE141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AF141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AG141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AH141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AI141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AJ141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AK141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AL141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AM141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AN141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AO141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AP141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AQ141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AR141" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="AS141" s="4"/>
       <c r="AT141" s="4"/>
@@ -15880,7 +15892,7 @@
       <c r="Y146" s="4"/>
       <c r="Z146" s="4"/>
       <c r="AA146" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="AB146" s="4"/>
       <c r="AC146" s="4"/>
@@ -15933,24 +15945,24 @@
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E147" s="4"/>
       <c r="F147" s="4"/>
       <c r="G147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="H147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="I147" s="4"/>
       <c r="J147" s="4"/>
@@ -15960,33 +15972,33 @@
       <c r="N147" s="4"/>
       <c r="O147" s="4"/>
       <c r="P147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="Q147" s="4"/>
       <c r="R147" s="4"/>
       <c r="S147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="T147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="U147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="V147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="W147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="X147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="Y147" s="4"/>
       <c r="Z147" s="4"/>
       <c r="AA147" s="4"/>
       <c r="AB147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AC147" s="4"/>
       <c r="AD147" s="3" t="s">
@@ -15996,33 +16008,33 @@
       <c r="AF147" s="4"/>
       <c r="AG147" s="4"/>
       <c r="AH147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AI147" s="4"/>
       <c r="AJ147" s="4"/>
       <c r="AK147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AL147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AM147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AN147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AO147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AP147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AQ147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AR147" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AS147" s="4"/>
       <c r="AT147" s="4"/>
@@ -16058,24 +16070,24 @@
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E148" s="4"/>
       <c r="F148" s="4"/>
       <c r="G148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="I148" s="4"/>
       <c r="J148" s="4"/>
@@ -16085,81 +16097,81 @@
       <c r="N148" s="4"/>
       <c r="O148" s="4"/>
       <c r="P148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="Q148" s="4"/>
       <c r="R148" s="4"/>
       <c r="S148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="T148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="U148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="V148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="W148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="X148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="Y148" s="4"/>
       <c r="Z148" s="4"/>
       <c r="AA148" s="4"/>
       <c r="AB148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AC148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AD148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AE148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AF148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AG148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AH148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AI148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AJ148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AK148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AL148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AM148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AN148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AO148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AP148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AQ148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AR148" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="AS148" s="4"/>
       <c r="AT148" s="4"/>
@@ -16195,24 +16207,24 @@
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E149" s="4"/>
       <c r="F149" s="4"/>
       <c r="G149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="I149" s="4"/>
       <c r="J149" s="4"/>
@@ -16222,79 +16234,79 @@
       <c r="N149" s="4"/>
       <c r="O149" s="4"/>
       <c r="P149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="Q149" s="4"/>
       <c r="R149" s="4"/>
       <c r="S149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="T149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="U149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="V149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="W149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="X149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="Y149" s="4"/>
       <c r="Z149" s="4"/>
       <c r="AA149" s="4"/>
       <c r="AB149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AC149" s="4"/>
       <c r="AD149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AE149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AF149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AG149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AH149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AI149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AJ149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AK149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AL149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AM149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AN149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AO149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AP149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AQ149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AR149" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="AS149" s="4"/>
       <c r="AT149" s="4"/>
@@ -16330,72 +16342,72 @@
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="I150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="J150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="K150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="L150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="M150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="N150" s="4"/>
       <c r="O150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="P150" s="4"/>
       <c r="Q150" s="4"/>
       <c r="R150" s="4"/>
       <c r="S150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="T150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="U150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="V150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="W150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="X150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="Y150" s="4"/>
       <c r="Z150" s="4"/>
       <c r="AA150" s="4"/>
       <c r="AB150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AC150" s="4"/>
       <c r="AD150" s="4"/>
@@ -16403,36 +16415,36 @@
       <c r="AF150" s="4"/>
       <c r="AG150" s="4"/>
       <c r="AH150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AI150" s="4"/>
       <c r="AJ150" s="4"/>
       <c r="AK150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AL150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AM150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AN150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AO150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AP150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AQ150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AR150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AS150" s="3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AT150" s="4"/>
       <c r="AU150" s="4"/>
@@ -16467,22 +16479,22 @@
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
       <c r="F151" s="4"/>
       <c r="G151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="I151" s="4"/>
       <c r="J151" s="4"/>
@@ -16495,28 +16507,28 @@
       <c r="Q151" s="4"/>
       <c r="R151" s="4"/>
       <c r="S151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="T151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="U151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="V151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="W151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="X151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="Y151" s="4"/>
       <c r="Z151" s="4"/>
       <c r="AA151" s="4"/>
       <c r="AB151" s="3" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="AC151" s="4"/>
       <c r="AD151" s="4"/>
@@ -16524,33 +16536,33 @@
       <c r="AF151" s="4"/>
       <c r="AG151" s="4"/>
       <c r="AH151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AI151" s="4"/>
       <c r="AJ151" s="4"/>
       <c r="AK151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AL151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AM151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AN151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AO151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AP151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AQ151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AR151" s="3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AS151" s="4"/>
       <c r="AT151" s="4"/>
@@ -16588,22 +16600,22 @@
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
       <c r="F152" s="4"/>
       <c r="G152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="H152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="I152" s="4"/>
       <c r="J152" s="4"/>
@@ -16616,28 +16628,28 @@
       <c r="Q152" s="4"/>
       <c r="R152" s="4"/>
       <c r="S152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="T152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="U152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="V152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="W152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="X152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="Y152" s="4"/>
       <c r="Z152" s="4"/>
       <c r="AA152" s="4"/>
       <c r="AB152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AC152" s="4"/>
       <c r="AD152" s="4"/>
@@ -16645,33 +16657,33 @@
       <c r="AF152" s="4"/>
       <c r="AG152" s="4"/>
       <c r="AH152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AI152" s="4"/>
       <c r="AJ152" s="4"/>
       <c r="AK152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AL152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AM152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AN152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AO152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AP152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AQ152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AR152" s="3" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="AS152" s="4"/>
       <c r="AT152" s="4"/>
@@ -16708,7 +16720,7 @@
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="4"/>
       <c r="B153" s="3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
@@ -16788,7 +16800,7 @@
       <c r="A154" s="4"/>
       <c r="B154" s="4"/>
       <c r="C154" s="3" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
@@ -16865,22 +16877,22 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
       <c r="F155" s="4"/>
       <c r="G155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="I155" s="4"/>
       <c r="J155" s="4"/>
@@ -16893,28 +16905,28 @@
       <c r="Q155" s="4"/>
       <c r="R155" s="4"/>
       <c r="S155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="T155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="U155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="V155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="W155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="X155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="Y155" s="4"/>
       <c r="Z155" s="4"/>
       <c r="AA155" s="4"/>
       <c r="AB155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AC155" s="4"/>
       <c r="AD155" s="4"/>
@@ -16922,33 +16934,33 @@
       <c r="AF155" s="4"/>
       <c r="AG155" s="4"/>
       <c r="AH155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AI155" s="4"/>
       <c r="AJ155" s="4"/>
       <c r="AK155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AL155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AM155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AN155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AO155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AP155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AQ155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AR155" s="3" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AS155" s="4"/>
       <c r="AT155" s="4"/>
@@ -17355,22 +17367,22 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D159" s="4"/>
       <c r="E159" s="4"/>
       <c r="F159" s="4"/>
       <c r="G159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="H159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="I159" s="4"/>
       <c r="J159" s="4"/>
@@ -17383,28 +17395,28 @@
       <c r="Q159" s="4"/>
       <c r="R159" s="4"/>
       <c r="S159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="T159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="U159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="V159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="W159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="X159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="Y159" s="4"/>
       <c r="Z159" s="4"/>
       <c r="AA159" s="4"/>
       <c r="AB159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AC159" s="4"/>
       <c r="AD159" s="4"/>
@@ -17412,33 +17424,33 @@
       <c r="AF159" s="4"/>
       <c r="AG159" s="4"/>
       <c r="AH159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AI159" s="4"/>
       <c r="AJ159" s="4"/>
       <c r="AK159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AL159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AM159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AN159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AO159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AP159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AQ159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AR159" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AS159" s="4"/>
       <c r="AT159" s="4"/>
@@ -17477,7 +17489,7 @@
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
       <c r="D160" s="3" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E160" s="4"/>
       <c r="F160" s="4"/>
@@ -17556,7 +17568,7 @@
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
       <c r="D161" s="3" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E161" s="4"/>
       <c r="F161" s="4"/>
@@ -17570,7 +17582,7 @@
       <c r="N161" s="4"/>
       <c r="O161" s="4"/>
       <c r="P161" s="3" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="Q161" s="4"/>
       <c r="R161" s="4"/>
@@ -17776,7 +17788,7 @@
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
       <c r="D163" s="3" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E163" s="4"/>
       <c r="F163" s="4"/>
@@ -17969,22 +17981,22 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D165" s="4"/>
       <c r="E165" s="4"/>
       <c r="F165" s="4"/>
       <c r="G165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="H165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I165" s="4"/>
       <c r="J165" s="4"/>
@@ -17997,28 +18009,28 @@
       <c r="Q165" s="4"/>
       <c r="R165" s="4"/>
       <c r="S165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="T165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="U165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="V165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="W165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="X165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="Y165" s="4"/>
       <c r="Z165" s="4"/>
       <c r="AA165" s="4"/>
       <c r="AB165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AC165" s="4"/>
       <c r="AD165" s="4"/>
@@ -18026,33 +18038,33 @@
       <c r="AF165" s="4"/>
       <c r="AG165" s="4"/>
       <c r="AH165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AI165" s="4"/>
       <c r="AJ165" s="4"/>
       <c r="AK165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AL165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AM165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AN165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AO165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AP165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AQ165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AR165" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AS165" s="4"/>
       <c r="AT165" s="4"/>
@@ -18089,7 +18101,7 @@
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="4"/>
       <c r="B166" s="3" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
@@ -18170,7 +18182,7 @@
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
       <c r="D167" s="3" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E167" s="4"/>
       <c r="F167" s="4"/>
@@ -18184,7 +18196,7 @@
       <c r="N167" s="4"/>
       <c r="O167" s="4"/>
       <c r="P167" s="3" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="Q167" s="4"/>
       <c r="R167" s="4"/>
@@ -18250,22 +18262,22 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D168" s="4"/>
       <c r="E168" s="4"/>
       <c r="F168" s="4"/>
       <c r="G168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="H168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="I168" s="4"/>
       <c r="J168" s="4"/>
@@ -18278,28 +18290,28 @@
       <c r="Q168" s="4"/>
       <c r="R168" s="4"/>
       <c r="S168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="T168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="U168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="V168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="W168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="X168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="Y168" s="4"/>
       <c r="Z168" s="4"/>
       <c r="AA168" s="4"/>
       <c r="AB168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AC168" s="4"/>
       <c r="AD168" s="4"/>
@@ -18307,33 +18319,33 @@
       <c r="AF168" s="4"/>
       <c r="AG168" s="4"/>
       <c r="AH168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AI168" s="4"/>
       <c r="AJ168" s="4"/>
       <c r="AK168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AL168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AM168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AN168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AO168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AP168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AQ168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AR168" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AS168" s="4"/>
       <c r="AT168" s="4"/>
@@ -18372,7 +18384,7 @@
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
       <c r="D169" s="3" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E169" s="4"/>
       <c r="F169" s="4"/>

</xml_diff>